<commit_message>
Refactored the `DataValidationView` to use `StudyLoader` instead of `call_command("load_study", ...)`.
Files checked in: DataRepo/data/tests/data_submission/accucor1.xlsx DataRepo/data/tests/data_submission/accucor2.xlsx DataRepo/data/tests/data_submission/animal_sample_good.xlsx DataRepo/data/tests/data_submission/animal_sample_unknown_researcher.xlsx DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx DataRepo/data/tests/submission_v3/study.xlsx DataRepo/tests/management/test_load_accucor_msruns.py DataRepo/tests/management/test_load_autoupdates.py DataRepo/tests/management/test_load_lcms_metadata.py DataRepo/tests/management/test_load_peak_annotations.py DataRepo/tests/management/test_studies_exporter.py DataRepo/tests/models/test_infusate.py DataRepo/tests/test_models.py DataRepo/tests/test_views.py DataRepo/tests/views/upload/test_validation.py DataRepo/views/upload/validation.py
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/data_submission/accucor1.xlsx
+++ b/DataRepo/data/tests/data_submission/accucor1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/data/tests/data_submission_good/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/data_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13D7D065-990D-5443-B624-878B9EC125AB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546012F4-ECCC-B940-BA33-34785539DF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="1500" windowWidth="47720" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="28">
   <si>
     <t>label</t>
   </si>
@@ -173,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,9 +213,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,26 +248,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,26 +283,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -932,7 +898,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -940,347 +906,6 @@
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>966.20992006516371</v>
-      </c>
-      <c r="E2">
-        <v>124298.52482949629</v>
-      </c>
-      <c r="F2">
-        <v>2106922.1289265431</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>393.34802059101128</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>8212.3083800777804</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>28395.53978609425</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1230.7350379833199</v>
-      </c>
-      <c r="E6">
-        <v>90053.998389199871</v>
-      </c>
-      <c r="F6">
-        <v>329490.63640371442</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>4910.4918336732862</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>6805.1776999919402</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0.99684543979009821</v>
-      </c>
-      <c r="F2">
-        <v>0.98292169992610812</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>3.1545602099017321E-3</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>3.831207619133086E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1.3247092454758819E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0.96566397124027548</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1.439156237216346E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1.994446638756105E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -1291,7 +916,7 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>15</v>
@@ -1314,26 +939,328 @@
         <v>966.20992006516371</v>
       </c>
       <c r="D2">
-        <v>124691.8728500873</v>
+        <v>124298.52482949629</v>
       </c>
       <c r="E2">
-        <v>2143529.977092715</v>
+        <v>2106922.1289265431</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>393.34802059101128</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>8212.3083800777804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>28395.53978609425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1230.7350379833199</v>
+      </c>
+      <c r="D6">
+        <v>90053.998389199871</v>
+      </c>
+      <c r="E6">
+        <v>329490.63640371442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>4910.4918336732862</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>6805.1776999919402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.99684543979009821</v>
+      </c>
+      <c r="E2">
+        <v>0.98292169992610812</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3.1545602099017321E-3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3.831207619133086E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1.3247092454758819E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.96566397124027548</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1.439156237216346E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1.994446638756105E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>966.20992006516371</v>
+      </c>
+      <c r="C2">
+        <v>124691.8728500873</v>
+      </c>
+      <c r="D2">
+        <v>2143529.977092715</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
         <v>1230.7350379833199</v>
       </c>
+      <c r="C3">
+        <v>90053.998389199871</v>
+      </c>
       <c r="D3">
-        <v>90053.998389199871</v>
-      </c>
-      <c r="E3">
         <v>341206.30593737972</v>
       </c>
     </row>

</xml_diff>